<commit_message>
Added hashmap to Board class for mapping algebraic coordinates to game board indexes Updated move toString, modified Board constructor, cleaned up code.
</commit_message>
<xml_diff>
--- a/120 Element array diagram.xlsx
+++ b/120 Element array diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnjmn\IdeaProjects\Tritogeneia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D349748-E0B4-47BA-9A71-267613303026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18B0931-92D9-4F03-BA0F-1C573D03FC74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0CD79BA7-1376-46AF-9251-8A763F46FD65}"/>
   </bookViews>
@@ -33,9 +33,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
-    <t>Single dimension array of 120 elements. 8 x 8 gameboard embedded in a 10 x 12 board. The extra row at the top and bottom are for checking if a knight goes out of bounds; an extra column on either side would be unnecessary, as this is a single dimension array and the squares on either side of the board, e.g. 39 and 40(ref. the board on the right), are contiguous. This structure is useful or bounds checking, but also prevents a piece from wrapping around the board.</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Single dimension array of 120 elements. 8 x 8 gameboard embedded in a 10 x 12 board. The extra row at the top and bottom are for checking if a knight goes out of bounds; an extra column on either side would be unnecessary, as this is a single dimension array and the squares on either side of the board, e.g. 39 and 40(ref. the center board), are contiguous. This structure is useful or bounds checking, but also prevents a piece from wrapping around the board.</t>
   </si>
 </sst>
 </file>
@@ -51,7 +75,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,12 +102,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -351,11 +381,129 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,7 +574,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -442,14 +589,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,14 +933,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF056B6B-C979-49D9-BD0A-119DF662D9CA}">
   <dimension ref="C1:AQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:AQ17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="3:43" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:43" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="1">
         <v>65</v>
       </c>
@@ -896,6 +1063,32 @@
       <c r="Z3" s="6">
         <v>19</v>
       </c>
+      <c r="AB3" s="34"/>
+      <c r="AC3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG3" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ3" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK3" s="39"/>
     </row>
     <row r="4" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="4">
@@ -958,6 +1151,36 @@
       <c r="Z4" s="6">
         <v>29</v>
       </c>
+      <c r="AB4" s="35">
+        <v>8</v>
+      </c>
+      <c r="AC4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="14">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="13">
+        <v>3</v>
+      </c>
+      <c r="AG4" s="14">
+        <v>4</v>
+      </c>
+      <c r="AH4" s="13">
+        <v>5</v>
+      </c>
+      <c r="AI4" s="14">
+        <v>6</v>
+      </c>
+      <c r="AJ4" s="15">
+        <v>7</v>
+      </c>
+      <c r="AK4" s="35">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="4">
@@ -1020,10 +1243,36 @@
       <c r="Z5" s="6">
         <v>39</v>
       </c>
-      <c r="AC5" s="31"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="24"/>
+      <c r="AB5" s="36">
+        <v>7</v>
+      </c>
+      <c r="AC5" s="16">
+        <v>8</v>
+      </c>
+      <c r="AD5" s="10">
+        <v>9</v>
+      </c>
+      <c r="AE5" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF5" s="10">
+        <v>11</v>
+      </c>
+      <c r="AG5" s="11">
+        <v>12</v>
+      </c>
+      <c r="AH5" s="10">
+        <v>13</v>
+      </c>
+      <c r="AI5" s="11">
+        <v>14</v>
+      </c>
+      <c r="AJ5" s="17">
+        <v>15</v>
+      </c>
+      <c r="AK5" s="36">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="4">
@@ -1086,6 +1335,36 @@
       <c r="Z6" s="6">
         <v>49</v>
       </c>
+      <c r="AB6" s="36">
+        <v>6</v>
+      </c>
+      <c r="AC6" s="18">
+        <v>16</v>
+      </c>
+      <c r="AD6" s="11">
+        <v>17</v>
+      </c>
+      <c r="AE6" s="10">
+        <v>18</v>
+      </c>
+      <c r="AF6" s="11">
+        <v>19</v>
+      </c>
+      <c r="AG6" s="10">
+        <v>20</v>
+      </c>
+      <c r="AH6" s="11">
+        <v>21</v>
+      </c>
+      <c r="AI6" s="10">
+        <v>22</v>
+      </c>
+      <c r="AJ6" s="19">
+        <v>23</v>
+      </c>
+      <c r="AK6" s="36">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E7" s="4">
@@ -1148,9 +1427,36 @@
       <c r="Z7" s="6">
         <v>59</v>
       </c>
-      <c r="AC7" s="24"/>
-      <c r="AE7" s="24"/>
-      <c r="AG7" s="24"/>
+      <c r="AB7" s="36">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="16">
+        <v>24</v>
+      </c>
+      <c r="AD7" s="10">
+        <v>25</v>
+      </c>
+      <c r="AE7" s="11">
+        <v>26</v>
+      </c>
+      <c r="AF7" s="10">
+        <v>27</v>
+      </c>
+      <c r="AG7" s="11">
+        <v>28</v>
+      </c>
+      <c r="AH7" s="10">
+        <v>29</v>
+      </c>
+      <c r="AI7" s="11">
+        <v>30</v>
+      </c>
+      <c r="AJ7" s="17">
+        <v>31</v>
+      </c>
+      <c r="AK7" s="36">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="4">
@@ -1213,6 +1519,36 @@
       <c r="Z8" s="6">
         <v>69</v>
       </c>
+      <c r="AB8" s="36">
+        <v>4</v>
+      </c>
+      <c r="AC8" s="18">
+        <v>32</v>
+      </c>
+      <c r="AD8" s="11">
+        <v>33</v>
+      </c>
+      <c r="AE8" s="10">
+        <v>34</v>
+      </c>
+      <c r="AF8" s="11">
+        <v>35</v>
+      </c>
+      <c r="AG8" s="10">
+        <v>36</v>
+      </c>
+      <c r="AH8" s="11">
+        <v>37</v>
+      </c>
+      <c r="AI8" s="10">
+        <v>38</v>
+      </c>
+      <c r="AJ8" s="19">
+        <v>39</v>
+      </c>
+      <c r="AK8" s="36">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E9" s="4">
@@ -1275,6 +1611,36 @@
       <c r="Z9" s="6">
         <v>79</v>
       </c>
+      <c r="AB9" s="36">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="16">
+        <v>40</v>
+      </c>
+      <c r="AD9" s="10">
+        <v>41</v>
+      </c>
+      <c r="AE9" s="11">
+        <v>42</v>
+      </c>
+      <c r="AF9" s="10">
+        <v>43</v>
+      </c>
+      <c r="AG9" s="11">
+        <v>44</v>
+      </c>
+      <c r="AH9" s="10">
+        <v>45</v>
+      </c>
+      <c r="AI9" s="11">
+        <v>46</v>
+      </c>
+      <c r="AJ9" s="17">
+        <v>47</v>
+      </c>
+      <c r="AK9" s="36">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="4">
@@ -1337,6 +1703,36 @@
       <c r="Z10" s="6">
         <v>89</v>
       </c>
+      <c r="AB10" s="36">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="18">
+        <v>48</v>
+      </c>
+      <c r="AD10" s="11">
+        <v>49</v>
+      </c>
+      <c r="AE10" s="10">
+        <v>50</v>
+      </c>
+      <c r="AF10" s="11">
+        <v>51</v>
+      </c>
+      <c r="AG10" s="10">
+        <v>52</v>
+      </c>
+      <c r="AH10" s="11">
+        <v>53</v>
+      </c>
+      <c r="AI10" s="10">
+        <v>54</v>
+      </c>
+      <c r="AJ10" s="19">
+        <v>55</v>
+      </c>
+      <c r="AK10" s="36">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="3:43" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" s="4">
@@ -1399,8 +1795,38 @@
       <c r="Z11" s="6">
         <v>99</v>
       </c>
+      <c r="AB11" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="20">
+        <v>56</v>
+      </c>
+      <c r="AD11" s="21">
+        <v>57</v>
+      </c>
+      <c r="AE11" s="22">
+        <v>58</v>
+      </c>
+      <c r="AF11" s="21">
+        <v>59</v>
+      </c>
+      <c r="AG11" s="22">
+        <v>60</v>
+      </c>
+      <c r="AH11" s="21">
+        <v>61</v>
+      </c>
+      <c r="AI11" s="22">
+        <v>62</v>
+      </c>
+      <c r="AJ11" s="23">
+        <v>63</v>
+      </c>
+      <c r="AK11" s="37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:43" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="4">
         <v>65</v>
       </c>
@@ -1461,6 +1887,32 @@
       <c r="Z12" s="6">
         <v>109</v>
       </c>
+      <c r="AB12" s="38"/>
+      <c r="AC12" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG12" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH12" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI12" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ12" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK12" s="40"/>
     </row>
     <row r="13" spans="3:43" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E13" s="7">
@@ -1526,215 +1978,215 @@
     </row>
     <row r="14" spans="3:43" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="3:43" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="25">
+      <c r="C15" s="24">
         <v>19</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="25">
         <v>20</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="26">
         <v>21</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="27">
         <v>22</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="26">
         <v>23</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <v>24</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="26">
         <v>25</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="27">
         <v>26</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K15" s="26">
         <v>27</v>
       </c>
-      <c r="L15" s="28">
+      <c r="L15" s="27">
         <v>28</v>
       </c>
-      <c r="M15" s="26">
+      <c r="M15" s="25">
         <v>29</v>
       </c>
-      <c r="N15" s="26">
+      <c r="N15" s="25">
         <v>30</v>
       </c>
-      <c r="O15" s="28">
+      <c r="O15" s="27">
         <v>31</v>
       </c>
-      <c r="P15" s="27">
+      <c r="P15" s="26">
         <v>32</v>
       </c>
-      <c r="Q15" s="28">
+      <c r="Q15" s="27">
         <v>33</v>
       </c>
-      <c r="R15" s="27">
+      <c r="R15" s="26">
         <v>34</v>
       </c>
-      <c r="S15" s="28">
+      <c r="S15" s="27">
         <v>35</v>
       </c>
-      <c r="T15" s="27">
+      <c r="T15" s="26">
         <v>36</v>
       </c>
-      <c r="U15" s="28">
+      <c r="U15" s="27">
         <v>37</v>
       </c>
-      <c r="V15" s="27">
+      <c r="V15" s="26">
         <v>38</v>
       </c>
-      <c r="W15" s="26">
+      <c r="W15" s="25">
         <v>39</v>
       </c>
-      <c r="X15" s="26">
+      <c r="X15" s="25">
         <v>40</v>
       </c>
-      <c r="Y15" s="27">
+      <c r="Y15" s="26">
         <v>41</v>
       </c>
-      <c r="Z15" s="28">
+      <c r="Z15" s="27">
         <v>42</v>
       </c>
-      <c r="AA15" s="27">
+      <c r="AA15" s="26">
         <v>43</v>
       </c>
-      <c r="AB15" s="28">
+      <c r="AB15" s="27">
         <v>44</v>
       </c>
-      <c r="AC15" s="27">
+      <c r="AC15" s="26">
         <v>45</v>
       </c>
-      <c r="AD15" s="28">
+      <c r="AD15" s="27">
         <v>46</v>
       </c>
-      <c r="AE15" s="27">
+      <c r="AE15" s="26">
         <v>47</v>
       </c>
-      <c r="AF15" s="28">
+      <c r="AF15" s="27">
         <v>48</v>
       </c>
-      <c r="AG15" s="26">
+      <c r="AG15" s="25">
         <v>49</v>
       </c>
-      <c r="AH15" s="26">
+      <c r="AH15" s="25">
         <v>50</v>
       </c>
-      <c r="AI15" s="28">
+      <c r="AI15" s="27">
         <v>51</v>
       </c>
-      <c r="AJ15" s="27">
+      <c r="AJ15" s="26">
         <v>52</v>
       </c>
-      <c r="AK15" s="28">
+      <c r="AK15" s="27">
         <v>53</v>
       </c>
-      <c r="AL15" s="27">
+      <c r="AL15" s="26">
         <v>54</v>
       </c>
-      <c r="AM15" s="28">
+      <c r="AM15" s="27">
         <v>55</v>
       </c>
-      <c r="AN15" s="27">
+      <c r="AN15" s="26">
         <v>56</v>
       </c>
-      <c r="AO15" s="28">
+      <c r="AO15" s="27">
         <v>57</v>
       </c>
-      <c r="AP15" s="27">
+      <c r="AP15" s="26">
         <v>58</v>
       </c>
-      <c r="AQ15" s="29">
+      <c r="AQ15" s="28">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="3:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="32"/>
-      <c r="W16" s="32"/>
-      <c r="X16" s="32"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="32"/>
-      <c r="AA16" s="32"/>
-      <c r="AB16" s="32"/>
-      <c r="AC16" s="32"/>
-      <c r="AD16" s="32"/>
-      <c r="AE16" s="32"/>
-      <c r="AF16" s="32"/>
-      <c r="AG16" s="32"/>
-      <c r="AH16" s="32"/>
-      <c r="AI16" s="32"/>
-      <c r="AJ16" s="32"/>
-      <c r="AK16" s="32"/>
-      <c r="AL16" s="32"/>
-      <c r="AM16" s="32"/>
-      <c r="AN16" s="32"/>
-      <c r="AO16" s="32"/>
-      <c r="AP16" s="32"/>
-      <c r="AQ16" s="32"/>
+      <c r="D16" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="29"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
+      <c r="AH16" s="29"/>
+      <c r="AI16" s="29"/>
+      <c r="AJ16" s="29"/>
+      <c r="AK16" s="29"/>
+      <c r="AL16" s="29"/>
+      <c r="AM16" s="29"/>
+      <c r="AN16" s="29"/>
+      <c r="AO16" s="29"/>
+      <c r="AP16" s="29"/>
+      <c r="AQ16" s="29"/>
     </row>
     <row r="17" spans="4:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="33"/>
-      <c r="U17" s="33"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="33"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="33"/>
-      <c r="AA17" s="33"/>
-      <c r="AB17" s="33"/>
-      <c r="AC17" s="33"/>
-      <c r="AD17" s="33"/>
-      <c r="AE17" s="33"/>
-      <c r="AF17" s="33"/>
-      <c r="AG17" s="33"/>
-      <c r="AH17" s="33"/>
-      <c r="AI17" s="33"/>
-      <c r="AJ17" s="33"/>
-      <c r="AK17" s="33"/>
-      <c r="AL17" s="33"/>
-      <c r="AM17" s="33"/>
-      <c r="AN17" s="33"/>
-      <c r="AO17" s="33"/>
-      <c r="AP17" s="33"/>
-      <c r="AQ17" s="33"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="30"/>
+      <c r="AD17" s="30"/>
+      <c r="AE17" s="30"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="30"/>
+      <c r="AI17" s="30"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="30"/>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="30"/>
+      <c r="AO17" s="30"/>
+      <c r="AP17" s="30"/>
+      <c r="AQ17" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>